<commit_message>
segunda tabela de vendas
</commit_message>
<xml_diff>
--- a/Dahboard_Vendas.xlsx
+++ b/Dahboard_Vendas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arquivos_Sistema\Downloads\projeto 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samara\Desktop\DIO\Dio_Bootcamp_Excel_IA\Dashboard_Vendas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BC4F395-8F07-4C81-B97E-AFF60C6E7897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F93E372-E4BF-4C4C-AA31-6E1FD5F549D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
   <sheets>
     <sheet name="A̳ssets" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="324">
   <si>
     <t>Paleta de Cores</t>
   </si>
@@ -1009,6 +1009,12 @@
   </si>
   <si>
     <t>Soma de EA Play Season Pass</t>
+  </si>
+  <si>
+    <t>Total de vendas Minecraft</t>
+  </si>
+  <si>
+    <t>Soma de Minecraft Season Pass Price</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1146,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1175,6 +1181,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -1182,44 +1189,6 @@
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-          <bgColor rgb="FF2AE6B1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="9"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF5BF6A8"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1262,17 +1231,55 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="0"/>
+          <bgColor rgb="FF2AE6B1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF5BF6A8"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="SlicerStyleLight6 2" pivot="0" table="0" count="10" xr9:uid="{6E85074E-4044-4685-93F8-CE3FB8A4436C}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF2AE6B1"/>
       <color rgb="FF5BF6A8"/>
-      <color rgb="FF2AE6B1"/>
       <color rgb="FF22C55E"/>
       <color rgb="FFE8E6E9"/>
       <color rgb="FF000000"/>
@@ -1705,12 +1712,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
+                    <a:srgbClr val="2AE6B1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1721,7 +1725,7 @@
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1762,6 +1766,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="2AE6B1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>C̳álculos!$B$7:$B$9</c:f>
@@ -1783,10 +1841,10 @@
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>217</c:v>
+                  <c:v>806</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1537</c:v>
+                  <c:v>1502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1922,8 +1980,6 @@
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
@@ -3273,115 +3329,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>154781</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>35718</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="6" name="Agrupar 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB4AA705-7986-7C37-9885-94929261E274}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="2238375" y="1369218"/>
-          <a:ext cx="5879306" cy="3488531"/>
-          <a:chOff x="2869407" y="1404937"/>
-          <a:chExt cx="5879306" cy="3488531"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Retângulo: Cantos Arredondados 4">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{584DEE9D-0B53-AB2A-36C8-53395A3638CE}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2869407" y="1404937"/>
-            <a:ext cx="5703093" cy="3488531"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="pt-BR" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:graphicFrame macro="">
-        <xdr:nvGraphicFramePr>
-          <xdr:cNvPr id="3" name="Gráfico 2">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FE35E9A-ADCF-48DC-AA2D-C5DD285F35B2}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGraphicFramePr>
-            <a:graphicFrameLocks/>
-          </xdr:cNvGraphicFramePr>
-        </xdr:nvGraphicFramePr>
-        <xdr:xfrm>
-          <a:off x="2976563" y="1571625"/>
-          <a:ext cx="5772150" cy="3271838"/>
-        </xdr:xfrm>
-        <a:graphic>
-          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-          </a:graphicData>
-        </a:graphic>
-      </xdr:graphicFrame>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -3395,8 +3342,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>159544</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Subscription Type">
@@ -3419,7 +3366,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3458,6 +3405,754 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>119061</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>34528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>559593</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>177403</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="13" name="Agrupar 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C48771C9-6C07-1FD4-B767-1A1CB08FED1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2202655" y="1237059"/>
+          <a:ext cx="5298282" cy="1285875"/>
+          <a:chOff x="2202655" y="1238250"/>
+          <a:chExt cx="4881563" cy="1143000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Retângulo: Cantos Arredondados 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39244152-6EF2-6938-0763-ED6F8A4F014C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2202657" y="1238250"/>
+            <a:ext cx="4869655" cy="1143000"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="5BF6A8"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="C̳álculos!E22">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Retângulo: Cantos Arredondados 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{502F9CD0-1C2F-463B-95BF-AB9BD65347F3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3178970" y="1681219"/>
+            <a:ext cx="3626104" cy="509532"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:fld id="{B4DF1D02-6FDC-467B-B426-5E1CDF12B398}" type="TxLink">
+              <a:rPr lang="en-US" sz="3200" b="0" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="5BF6A8"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos Narrow"/>
+              </a:rPr>
+              <a:pPr algn="ctr"/>
+              <a:t> R$ 990,00 </a:t>
+            </a:fld>
+            <a:endParaRPr lang="pt-BR" sz="3200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="5BF6A8"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="11" name="Imagem 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED75EE7F-C4DD-4D82-ACE0-5D4351E85D9C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2440782" y="1535905"/>
+            <a:ext cx="785812" cy="785812"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="Retângulo: Cantos Superiores Arredondados 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F719435C-E27F-534A-FA9D-9C7511280FEE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2202655" y="1238250"/>
+            <a:ext cx="4881563" cy="345281"/>
+          </a:xfrm>
+          <a:prstGeom prst="round2SameRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="2AE6B1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>TOTAL DE VENDAS EA PLAY</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>164304</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>34528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>164305</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>177403</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="23" name="Agrupar 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ED41468-590B-DCE2-8830-E7B670D52B4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7712867" y="1237059"/>
+          <a:ext cx="5298282" cy="1285875"/>
+          <a:chOff x="7712867" y="1235868"/>
+          <a:chExt cx="5298282" cy="1285875"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Retângulo: Cantos Arredondados 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E963A6-E97F-C9B7-4004-0F0BF36A1EE2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7712869" y="1235868"/>
+            <a:ext cx="5285357" cy="1285875"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="5BF6A8"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="C̳álculos!E33">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="Retângulo: Cantos Arredondados 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB69EAEF-222D-FFCC-9DAA-BFEECA3EC134}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8689183" y="1734207"/>
+            <a:ext cx="3935650" cy="573224"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:fld id="{AA0BA186-B814-404C-9A7A-54006A759D92}" type="TxLink">
+              <a:rPr lang="en-US" sz="3200" b="0" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="5BF6A8"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> R$ 1.140,00 </a:t>
+            </a:fld>
+            <a:endParaRPr lang="pt-BR" sz="3200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="5BF6A8"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="Retângulo: Cantos Superiores Arredondados 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23E22B62-CE92-881B-F723-8D2844095877}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7712867" y="1235868"/>
+            <a:ext cx="5298282" cy="388441"/>
+          </a:xfrm>
+          <a:prstGeom prst="round2SameRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="2AE6B1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>TOTAL DE VENDAS MINECRAFT</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="20" name="Agrupar 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{621BDB92-4230-471E-AEEF-EE5C759AD596}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="7989094" y="1785937"/>
+            <a:ext cx="1190625" cy="559594"/>
+            <a:chOff x="3495675" y="5400674"/>
+            <a:chExt cx="1549476" cy="752476"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="21" name="Imagem 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB25FCF-1D8E-5882-865F-02B43FB63E56}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3998608" y="5400674"/>
+              <a:ext cx="555497" cy="609599"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="22" name="Gráfico 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23306593-19C6-140E-0EC5-6D1B66250000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+              <a:extLst>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId5"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3495675" y="5895937"/>
+              <a:ext cx="1549476" cy="257213"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>130970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>83343</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="Agrupar 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD489884-14CE-8C80-3773-3A10751E6E51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2178843" y="2857501"/>
+          <a:ext cx="11358563" cy="3521867"/>
+          <a:chOff x="2178843" y="2857501"/>
+          <a:chExt cx="11358563" cy="3521867"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="6" name="Agrupar 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB4AA705-7986-7C37-9885-94929261E274}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2190750" y="2869404"/>
+            <a:ext cx="11346656" cy="3509964"/>
+            <a:chOff x="2809876" y="1333499"/>
+            <a:chExt cx="5938837" cy="3509964"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="Retângulo: Cantos Arredondados 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{584DEE9D-0B53-AB2A-36C8-53395A3638CE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2809876" y="1333499"/>
+              <a:ext cx="5703093" cy="3488531"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="15000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Gráfico 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FE35E9A-ADCF-48DC-AA2D-C5DD285F35B2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="2976563" y="1571625"/>
+            <a:ext cx="5772150" cy="3271838"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="Retângulo: Cantos Superiores Arredondados 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ED6C1EF-6753-442B-9D2F-ED424A1127CC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2178843" y="2857501"/>
+            <a:ext cx="10906125" cy="575368"/>
+          </a:xfrm>
+          <a:prstGeom prst="round2SameRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="2AE6B1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>TOTAL DE SUBSCRIPTION XBOX</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1" baseline="0">
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> GAME PASS</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200" b="1">
+              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8243,7 +8938,373 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A4A3EDE5-C29E-4A4E-85BD-6E8AB1E26CD2}" name="Tabela dinâmica2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C95670A8-DAA0-4FB2-A19A-702512F30FAF}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="B29:C33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="281">
+        <item x="87"/>
+        <item x="61"/>
+        <item x="206"/>
+        <item x="275"/>
+        <item x="112"/>
+        <item x="228"/>
+        <item x="35"/>
+        <item x="253"/>
+        <item x="136"/>
+        <item x="3"/>
+        <item x="161"/>
+        <item x="185"/>
+        <item x="7"/>
+        <item x="88"/>
+        <item x="16"/>
+        <item x="186"/>
+        <item x="162"/>
+        <item x="276"/>
+        <item x="36"/>
+        <item x="254"/>
+        <item x="207"/>
+        <item x="137"/>
+        <item x="62"/>
+        <item x="9"/>
+        <item x="113"/>
+        <item x="229"/>
+        <item x="163"/>
+        <item x="15"/>
+        <item x="6"/>
+        <item x="63"/>
+        <item x="37"/>
+        <item x="230"/>
+        <item x="255"/>
+        <item x="277"/>
+        <item x="138"/>
+        <item x="89"/>
+        <item x="114"/>
+        <item x="17"/>
+        <item x="187"/>
+        <item x="90"/>
+        <item x="139"/>
+        <item x="18"/>
+        <item x="38"/>
+        <item x="64"/>
+        <item x="231"/>
+        <item x="208"/>
+        <item x="256"/>
+        <item x="278"/>
+        <item x="13"/>
+        <item x="115"/>
+        <item x="164"/>
+        <item x="91"/>
+        <item x="188"/>
+        <item x="19"/>
+        <item x="209"/>
+        <item x="116"/>
+        <item x="257"/>
+        <item x="279"/>
+        <item x="140"/>
+        <item x="65"/>
+        <item x="39"/>
+        <item x="92"/>
+        <item x="210"/>
+        <item x="141"/>
+        <item x="232"/>
+        <item x="258"/>
+        <item x="40"/>
+        <item x="66"/>
+        <item x="117"/>
+        <item x="5"/>
+        <item x="165"/>
+        <item x="14"/>
+        <item x="67"/>
+        <item x="211"/>
+        <item x="189"/>
+        <item x="259"/>
+        <item x="20"/>
+        <item x="93"/>
+        <item x="233"/>
+        <item x="41"/>
+        <item x="142"/>
+        <item x="166"/>
+        <item x="143"/>
+        <item x="94"/>
+        <item x="212"/>
+        <item x="167"/>
+        <item x="68"/>
+        <item x="42"/>
+        <item x="234"/>
+        <item x="118"/>
+        <item x="21"/>
+        <item x="260"/>
+        <item x="144"/>
+        <item x="190"/>
+        <item x="213"/>
+        <item x="168"/>
+        <item x="43"/>
+        <item x="235"/>
+        <item x="119"/>
+        <item x="95"/>
+        <item x="22"/>
+        <item x="69"/>
+        <item x="145"/>
+        <item x="191"/>
+        <item x="169"/>
+        <item x="120"/>
+        <item x="261"/>
+        <item x="96"/>
+        <item x="236"/>
+        <item x="0"/>
+        <item x="23"/>
+        <item x="44"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="97"/>
+        <item x="170"/>
+        <item x="262"/>
+        <item x="237"/>
+        <item x="146"/>
+        <item x="45"/>
+        <item x="24"/>
+        <item x="121"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="192"/>
+        <item x="72"/>
+        <item x="263"/>
+        <item x="171"/>
+        <item x="238"/>
+        <item x="46"/>
+        <item x="98"/>
+        <item x="214"/>
+        <item x="147"/>
+        <item x="193"/>
+        <item x="264"/>
+        <item x="99"/>
+        <item x="172"/>
+        <item x="47"/>
+        <item x="122"/>
+        <item x="11"/>
+        <item x="239"/>
+        <item x="148"/>
+        <item x="215"/>
+        <item x="1"/>
+        <item x="25"/>
+        <item x="73"/>
+        <item x="123"/>
+        <item x="216"/>
+        <item x="265"/>
+        <item x="149"/>
+        <item x="240"/>
+        <item x="194"/>
+        <item x="26"/>
+        <item x="48"/>
+        <item x="173"/>
+        <item x="100"/>
+        <item x="74"/>
+        <item x="195"/>
+        <item x="174"/>
+        <item x="124"/>
+        <item x="241"/>
+        <item x="266"/>
+        <item x="49"/>
+        <item x="101"/>
+        <item x="150"/>
+        <item x="217"/>
+        <item x="75"/>
+        <item x="27"/>
+        <item x="151"/>
+        <item x="102"/>
+        <item x="218"/>
+        <item x="242"/>
+        <item x="267"/>
+        <item x="125"/>
+        <item x="50"/>
+        <item x="28"/>
+        <item x="76"/>
+        <item x="196"/>
+        <item x="175"/>
+        <item x="4"/>
+        <item x="126"/>
+        <item x="219"/>
+        <item x="268"/>
+        <item x="77"/>
+        <item x="51"/>
+        <item x="152"/>
+        <item x="243"/>
+        <item x="127"/>
+        <item x="103"/>
+        <item x="244"/>
+        <item x="29"/>
+        <item x="197"/>
+        <item x="176"/>
+        <item x="78"/>
+        <item x="269"/>
+        <item x="52"/>
+        <item x="153"/>
+        <item x="10"/>
+        <item x="79"/>
+        <item x="104"/>
+        <item x="30"/>
+        <item x="177"/>
+        <item x="220"/>
+        <item x="245"/>
+        <item x="270"/>
+        <item x="128"/>
+        <item x="8"/>
+        <item x="154"/>
+        <item x="198"/>
+        <item x="53"/>
+        <item x="31"/>
+        <item x="271"/>
+        <item x="246"/>
+        <item x="105"/>
+        <item x="178"/>
+        <item x="221"/>
+        <item x="80"/>
+        <item x="129"/>
+        <item x="155"/>
+        <item x="54"/>
+        <item x="199"/>
+        <item x="247"/>
+        <item x="55"/>
+        <item x="106"/>
+        <item x="179"/>
+        <item x="81"/>
+        <item x="156"/>
+        <item x="222"/>
+        <item x="200"/>
+        <item x="130"/>
+        <item x="248"/>
+        <item x="56"/>
+        <item x="223"/>
+        <item x="157"/>
+        <item x="131"/>
+        <item x="180"/>
+        <item x="201"/>
+        <item x="82"/>
+        <item x="107"/>
+        <item x="32"/>
+        <item x="158"/>
+        <item x="132"/>
+        <item x="202"/>
+        <item x="83"/>
+        <item x="181"/>
+        <item x="224"/>
+        <item x="249"/>
+        <item x="57"/>
+        <item x="108"/>
+        <item x="203"/>
+        <item x="133"/>
+        <item x="225"/>
+        <item x="109"/>
+        <item x="272"/>
+        <item x="182"/>
+        <item x="84"/>
+        <item x="250"/>
+        <item x="58"/>
+        <item x="110"/>
+        <item x="59"/>
+        <item x="183"/>
+        <item x="226"/>
+        <item x="85"/>
+        <item x="273"/>
+        <item x="159"/>
+        <item x="33"/>
+        <item x="204"/>
+        <item x="251"/>
+        <item x="134"/>
+        <item x="205"/>
+        <item x="60"/>
+        <item x="184"/>
+        <item x="160"/>
+        <item x="274"/>
+        <item x="227"/>
+        <item x="135"/>
+        <item x="86"/>
+        <item x="34"/>
+        <item x="252"/>
+        <item x="111"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="6" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Soma de Minecraft Season Pass Price" fld="10" baseField="0" baseItem="0" numFmtId="44"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A4A3EDE5-C29E-4A4E-85BD-6E8AB1E26CD2}" name="Tab_EA_total" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B18:C22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -8591,7 +9652,7 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="6" item="0" hier="-1"/>
+    <pageField fld="6" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Soma de EA Play Season Pass" fld="8" baseField="2" baseItem="0"/>
@@ -8608,8 +9669,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C3E645B6-6B7E-4CFC-9901-E567F4EA015F}" name="Tbl_Total" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C3E645B6-6B7E-4CFC-9901-E567F4EA015F}" name="Tbl_Total" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="B6:C9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -8941,7 +10002,7 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="6" item="0" hier="-1"/>
+    <pageField fld="6" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Soma de Total Value" fld="12" baseField="0" baseItem="0" numFmtId="44"/>
@@ -8973,14 +10034,15 @@
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Subscription_Type" xr10:uid="{2F4C8FA2-8F0D-4074-8748-0E278A4E485C}" sourceName="Subscription Type">
   <pivotTables>
     <pivotTable tabId="3" name="Tbl_Total"/>
-    <pivotTable tabId="3" name="Tabela dinâmica2"/>
+    <pivotTable tabId="3" name="Tab_EA_total"/>
+    <pivotTable tabId="3" name="Tabela dinâmica1"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="386785422">
       <items count="3">
-        <i x="1" s="1"/>
+        <i x="1"/>
         <i x="0"/>
-        <i x="2"/>
+        <i x="2" s="1"/>
       </items>
     </tabular>
   </data>
@@ -8994,7 +10056,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="13">
   <autoFilter ref="A1:M296" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}">
     <filterColumn colId="7">
       <filters>
@@ -9003,19 +10065,19 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="9" dataCellStyle="Moeda"/>
-    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="6" dataCellStyle="Moeda"/>
-    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="4" dataCellStyle="Moeda"/>
-    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="3" dataCellStyle="Moeda"/>
-    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="2" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="7" dataCellStyle="Moeda"/>
+    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="4" dataCellStyle="Moeda"/>
+    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="2" dataCellStyle="Moeda"/>
+    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="1" dataCellStyle="Moeda"/>
+    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="0" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9516,8 +10578,8 @@
   </sheetPr>
   <dimension ref="A1:M296"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R50" sqref="R50"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21687,18 +22749,18 @@
   <sheetPr>
     <tabColor theme="3" tint="0.749992370372631"/>
   </sheetPr>
-  <dimension ref="B2:C22"/>
+  <dimension ref="B2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.42578125" customWidth="1"/>
@@ -21728,7 +22790,7 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -21744,7 +22806,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="14">
-        <v>217</v>
+        <v>806</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -21752,7 +22814,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="14">
-        <v>1537</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -21760,7 +22822,7 @@
         <v>314</v>
       </c>
       <c r="C9" s="14">
-        <v>1754</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
@@ -21773,10 +22835,10 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>313</v>
       </c>
@@ -21784,7 +22846,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>22</v>
       </c>
@@ -21792,7 +22854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>26</v>
       </c>
@@ -21800,20 +22862,82 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="19">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>314</v>
       </c>
       <c r="C22" s="19">
-        <v>600</v>
+        <v>990</v>
+      </c>
+      <c r="E22" s="20">
+        <f>GETPIVOTDATA("EA Play Season Pass
+Price",$B$18)</f>
+        <v>990</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C29" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="14">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="14">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="C33" s="14">
+        <v>1140</v>
+      </c>
+      <c r="E33" s="20">
+        <f>GETPIVOTDATA("Minecraft Season Pass Price",$B$29)</f>
+        <v>1140</v>
       </c>
     </row>
   </sheetData>
@@ -21821,7 +22945,7 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -21829,8 +22953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210F14EF-C0B7-459D-9E09-3130BA4314A6}">
   <dimension ref="A1:Q201"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22469,6 +23593,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
@@ -22477,15 +23610,6 @@
     <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22744,20 +23868,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD3D529-BCD3-4ECD-9B2A-42924892FFCB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
     <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>